<commit_message>
Corrected db link, wrote code for generating test results
</commit_message>
<xml_diff>
--- a/Testing/Book1_results.xlsx
+++ b/Testing/Book1_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,11 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Generated Result</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Generated Answer</t>
         </is>
       </c>
@@ -476,15 +481,20 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>SELECT city_name, MAX(population) FROM city WHERE state_name = "arizona"</t>
+          <t>SELECT city_name FROM city WHERE state_name = "arizona" ORDER BY population DESC LIMIT 1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>phoenix</t>
+          <t>[('phoenix',)]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
+        <is>
+          <t>[('phoenix',)]</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Phoenix</t>
         </is>
@@ -511,10 +521,15 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>delaware, allegheny, hudson</t>
+          <t>[('delaware',), ('allegheny',), ('hudson',)]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
+        <is>
+          <t>[('delaware',), ('allegheny',), ('hudson',)]</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>delaware, allegheny, hudson</t>
         </is>
@@ -541,10 +556,15 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>266807.0</t>
+          <t>[(266807.0,)]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
+        <is>
+          <t>[(266807.0,)]</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>266807.0</t>
         </is>
@@ -571,10 +591,15 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>4113200</t>
+          <t>[(4113200,)]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
+        <is>
+          <t>[(4113200,)]</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>4113200</t>
         </is>

</xml_diff>

<commit_message>
Added accuracy code, modified front end and corrected test data set
</commit_message>
<xml_diff>
--- a/Testing/Book1_results.xlsx
+++ b/Testing/Book1_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,32 +471,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>what is the biggest city in arizona</t>
+          <t>count the states which have elevations lower than what alabama has</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SELECT city.city_name FROM city WHERE city.state_name='arizona' AND city.population=(SELECT max(city.population) FROM city WHERE city.state_name='arizona');</t>
+          <t>select count(highlow.state_name) from highlow where highlow.lowest_elevation &lt;(select highlow.lowest_elevation from highlow where highlow.state_name='alabama');</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>SELECT city_name FROM city WHERE state_name = "arizona" ORDER BY population DESC LIMIT 1</t>
+          <t>SELECT COUNT(*) FROM highlow WHERE CAST(lowest_elevation AS INTEGER) &lt; (SELECT CAST(lowest_elevation AS INTEGER) FROM highlow WHERE state_name = "alabama")</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[('phoenix',)]</t>
+          <t>(2,)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[('phoenix',)]</t>
+          <t>(2,)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -506,32 +506,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>which rivers run through the state with the largest city in the us ?</t>
+          <t>give me the number of rivers in california</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SELECT river.river_name FROM river WHERE river.traverse IN (SELECT city.state_name FROM city WHERE city.population = (SELECT max(city.population) FROM city));</t>
+          <t>select count(river.river_name) from river where river.traverse='california';</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>SELECT river_name FROM river WHERE traverse IN (SELECT city_name FROM city WHERE population = (SELECT MAX(population) FROM city))</t>
+          <t>SELECT COUNT(*) FROM river WHERE traverse = 'california'</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[('delaware',), ('allegheny',), ('hudson',)]</t>
+          <t>(1,)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[('delaware',), ('allegheny',), ('hudson',)]</t>
+          <t>(1,)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>delaware, allegheny, hudson</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -541,32 +541,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>how big is texas</t>
+          <t>give me the states that border utah</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SELECT state.area FROM state WHERE state.state_name='texas';</t>
+          <t>select border_info.border from border_info where border_info.state_name='utah';</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>SELECT area FROM state WHERE state_name = "texas"</t>
+          <t>SELECT state_name FROM border_info WHERE border = 'utah' LIMIT 5</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[(266807.0,)]</t>
+          <t>('wyoming',)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[(266807.0,)]</t>
+          <t>('wyoming',)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>266807.0</t>
+          <t>arizona, colorado, idaho, nevada, new mexico</t>
         </is>
       </c>
     </row>
@@ -576,32 +576,553 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>how many people live in washington</t>
+          <t>how high is mount mckinley</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SELECT state.population FROM state WHERE state.state_name='washington';</t>
+          <t>select highlow.highest_elevation from highlow where highlow.highest_point='mount mckinley';</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>SELECT population FROM state WHERE state_name = "washington"</t>
+          <t>SELECT mountain_altitude FROM mountain WHERE mountain_name = "mckinley"</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[(4113200,)]</t>
+          <t>('6194',)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[(4113200,)]</t>
+          <t>('6194',)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>4113200</t>
+          <t>6194</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>how high is the highest point in america</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>select max(highlow.highest_elevation) from highlow;</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>SELECT MAX(mountain_altitude) AS "highest_point" FROM mountain</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>('979',)</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>('979',)</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>6194</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>how high is the highest point of alabama</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>select highlow.highest_elevation from highlow where highlow.state_name='alabama';</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>SELECT "highest_point" FROM highlow WHERE state_name = "alabama"</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>('734',)</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>('734',)</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>cheaha mountain</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>how large is alaska</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>select state.area from state where state.state_name='alaska';</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>SELECT area FROM state WHERE state_name = "alaska"</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>(591000.0,)</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>(591000.0,)</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>591000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>how large is texas</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>select state.area from state where state.state_name='texas';</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>SELECT area FROM state WHERE state_name = "texas"</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>(266807.0,)</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>(266807.0,)</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>266807.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>how long is the colorado river</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>select river.length from river where river.river_name='colorado';</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>SELECT length FROM river WHERE river_name = "colorado" AND traverse = "usa"</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>(2333,)</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>how long is the delaware river</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>select river.length from river where river.river_name='delaware';</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>SELECT length FROM river WHERE river_name = "delaware" AND traverse = "pennsylvania"</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>(451,)</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>(451,)</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>451 miles</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>how long is the longest river in california</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>select river.length from river where river.traverse='california' and river.length=(select max(river.length) from river where river.traverse='california');</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>SELECT MAX(length) FROM river WHERE traverse = 'california'</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>(2333,)</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>(2333,)</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2333</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>how long is the longest river in the usa</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>select river.length from river where river.length=(select max(river.length) from river);</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>SELECT MAX(length) FROM river WHERE country_name = "usa"</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>(3968,)</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>(3968,)</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>3968</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>how long is the north platte river</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>select river.length from river where river.river_name='north platte';</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>SELECT length FROM river WHERE river_name = "north platte"</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>(1094,)</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>(1094,)</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1094 miles</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>how long is the ohio river</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>select river.length from river where river.river_name='ohio';</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>SELECT length FROM river WHERE river_name = "ohio" LIMIT 5</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>(1569,)</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>(1569,)</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>The Ohio River is 1569 miles long.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>how many capitals does rhode island have</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>select count(state.capital) from state where state.state_name='rhode island';</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>SELECT COUNT(capital) FROM state WHERE state_name = "rhode island"</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>(1,)</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>(1,)</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>how many cities are there in the united states</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>select count(city.city_name) from city;</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>SELECT COUNT(*) FROM city WHERE country_name = 'usa'</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>(386,)</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>(386,)</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>386</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>how many citizens does the biggest city have in the usa</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>select city.population from city where city.population=(select max(city.population) from city);</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>SELECT MAX(population) FROM city WHERE country_name = 'usa'</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>(7071639,)</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>(7071639,)</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>7071639</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>how many colorado rivers are there</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>select count(river.river_name) from river where river.river_name='colorado';</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>SELECT COUNT(*) FROM river WHERE river_name = 'colorado'</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>(5,)</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>(5,)</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>how many people lived in austin</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>select city.population from city where city.city_name='austin';</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>SELECT population FROM city WHERE city_name = "austin" LIMIT 5</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>(345496,)</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>(345496,)</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>345496</t>
         </is>
       </c>
     </row>

</xml_diff>